<commit_message>
Updates to Note to fix URL issues. Added tests.
</commit_message>
<xml_diff>
--- a/notedb/tests/test_files/test_template_format_1.xlsx
+++ b/notedb/tests/test_files/test_template_format_1.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>state</t>
   </si>
@@ -42,10 +42,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,13 +76,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -447,12 +458,367 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E2, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F2, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G2, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E3, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F3, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G3, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E4, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F4, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G4, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E5, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F5, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G5, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E6, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F6, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G6, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E7, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F7, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G7, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E8, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F8, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G8, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E9, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F9, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G9, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E10, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F10, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G10, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E11, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F11, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G11, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E12, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F12, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G12, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E13, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F13, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G13, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E14, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F14, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G14, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E15, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F15, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G15, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E16, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F16, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G16, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E17, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F17, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G17, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E18, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F18, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G18, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E19, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F19, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G19, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E20, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F20, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G20, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E21, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F21, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G21, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E22, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F22, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G22, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E23, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F23, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G23, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E24, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F24, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G24, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="str">
+        <f>HYPERLINK(Sheet1!E25, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f>HYPERLINK(Sheet1!F25, "link")</f>
+        <v>link</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f>HYPERLINK(Sheet1!G25, "link")</f>
+        <v>link</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created the Database class. Updated tool with database connection.
Also added unit tests for database.
Tool can also run if database is not available.
</commit_message>
<xml_diff>
--- a/notedb/tests/test_files/test_template_format_1.xlsx
+++ b/notedb/tests/test_files/test_template_format_1.xlsx
@@ -461,7 +461,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,338 +484,338 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E2, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E2)),HYPERLINK(Sheet1!E2, "link"),"")</f>
+        <v/>
       </c>
       <c r="B2" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F2, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F2)),HYPERLINK(Sheet1!F2, "link"),"")</f>
+        <v/>
       </c>
       <c r="C2" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G2, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G2)),HYPERLINK(Sheet1!G2, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E3, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E3)),HYPERLINK(Sheet1!E3, "link"),"")</f>
+        <v/>
       </c>
       <c r="B3" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F3, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F3)),HYPERLINK(Sheet1!F3, "link"),"")</f>
+        <v/>
       </c>
       <c r="C3" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G3, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G3)),HYPERLINK(Sheet1!G3, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E4, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E4)),HYPERLINK(Sheet1!E4, "link"),"")</f>
+        <v/>
       </c>
       <c r="B4" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F4, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F4)),HYPERLINK(Sheet1!F4, "link"),"")</f>
+        <v/>
       </c>
       <c r="C4" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G4, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G4)),HYPERLINK(Sheet1!G4, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E5, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E5)),HYPERLINK(Sheet1!E5, "link"),"")</f>
+        <v/>
       </c>
       <c r="B5" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F5, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F5)),HYPERLINK(Sheet1!F5, "link"),"")</f>
+        <v/>
       </c>
       <c r="C5" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G5, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G5)),HYPERLINK(Sheet1!G5, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E6, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E6)),HYPERLINK(Sheet1!E6, "link"),"")</f>
+        <v/>
       </c>
       <c r="B6" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F6, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F6)),HYPERLINK(Sheet1!F6, "link"),"")</f>
+        <v/>
       </c>
       <c r="C6" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G6, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G6)),HYPERLINK(Sheet1!G6, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E7, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E7)),HYPERLINK(Sheet1!E7, "link"),"")</f>
+        <v/>
       </c>
       <c r="B7" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F7, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F7)),HYPERLINK(Sheet1!F7, "link"),"")</f>
+        <v/>
       </c>
       <c r="C7" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G7, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G7)),HYPERLINK(Sheet1!G7, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E8, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E8)),HYPERLINK(Sheet1!E8, "link"),"")</f>
+        <v/>
       </c>
       <c r="B8" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F8, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F8)),HYPERLINK(Sheet1!F8, "link"),"")</f>
+        <v/>
       </c>
       <c r="C8" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G8, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G8)),HYPERLINK(Sheet1!G8, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E9, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E9)),HYPERLINK(Sheet1!E9, "link"),"")</f>
+        <v/>
       </c>
       <c r="B9" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F9, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F9)),HYPERLINK(Sheet1!F9, "link"),"")</f>
+        <v/>
       </c>
       <c r="C9" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G9, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G9)),HYPERLINK(Sheet1!G9, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E10, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E10)),HYPERLINK(Sheet1!E10, "link"),"")</f>
+        <v/>
       </c>
       <c r="B10" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F10, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F10)),HYPERLINK(Sheet1!F10, "link"),"")</f>
+        <v/>
       </c>
       <c r="C10" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G10, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G10)),HYPERLINK(Sheet1!G10, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E11, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E11)),HYPERLINK(Sheet1!E11, "link"),"")</f>
+        <v/>
       </c>
       <c r="B11" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F11, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F11)),HYPERLINK(Sheet1!F11, "link"),"")</f>
+        <v/>
       </c>
       <c r="C11" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G11, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G11)),HYPERLINK(Sheet1!G11, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E12, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E12)),HYPERLINK(Sheet1!E12, "link"),"")</f>
+        <v/>
       </c>
       <c r="B12" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F12, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F12)),HYPERLINK(Sheet1!F12, "link"),"")</f>
+        <v/>
       </c>
       <c r="C12" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G12, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G12)),HYPERLINK(Sheet1!G12, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E13, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E13)),HYPERLINK(Sheet1!E13, "link"),"")</f>
+        <v/>
       </c>
       <c r="B13" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F13, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F13)),HYPERLINK(Sheet1!F13, "link"),"")</f>
+        <v/>
       </c>
       <c r="C13" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G13, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G13)),HYPERLINK(Sheet1!G13, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E14, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E14)),HYPERLINK(Sheet1!E14, "link"),"")</f>
+        <v/>
       </c>
       <c r="B14" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F14, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F14)),HYPERLINK(Sheet1!F14, "link"),"")</f>
+        <v/>
       </c>
       <c r="C14" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G14, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G14)),HYPERLINK(Sheet1!G14, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E15, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E15)),HYPERLINK(Sheet1!E15, "link"),"")</f>
+        <v/>
       </c>
       <c r="B15" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F15, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F15)),HYPERLINK(Sheet1!F15, "link"),"")</f>
+        <v/>
       </c>
       <c r="C15" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G15, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G15)),HYPERLINK(Sheet1!G15, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E16, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E16)),HYPERLINK(Sheet1!E16, "link"),"")</f>
+        <v/>
       </c>
       <c r="B16" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F16, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F16)),HYPERLINK(Sheet1!F16, "link"),"")</f>
+        <v/>
       </c>
       <c r="C16" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G16, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G16)),HYPERLINK(Sheet1!G16, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E17, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E17)),HYPERLINK(Sheet1!E17, "link"),"")</f>
+        <v/>
       </c>
       <c r="B17" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F17, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F17)),HYPERLINK(Sheet1!F17, "link"),"")</f>
+        <v/>
       </c>
       <c r="C17" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G17, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G17)),HYPERLINK(Sheet1!G17, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E18, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E18)),HYPERLINK(Sheet1!E18, "link"),"")</f>
+        <v/>
       </c>
       <c r="B18" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F18, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F18)),HYPERLINK(Sheet1!F18, "link"),"")</f>
+        <v/>
       </c>
       <c r="C18" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G18, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G18)),HYPERLINK(Sheet1!G18, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E19, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E19)),HYPERLINK(Sheet1!E19, "link"),"")</f>
+        <v/>
       </c>
       <c r="B19" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F19, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F19)),HYPERLINK(Sheet1!F19, "link"),"")</f>
+        <v/>
       </c>
       <c r="C19" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G19, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G19)),HYPERLINK(Sheet1!G19, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E20, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E20)),HYPERLINK(Sheet1!E20, "link"),"")</f>
+        <v/>
       </c>
       <c r="B20" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F20, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F20)),HYPERLINK(Sheet1!F20, "link"),"")</f>
+        <v/>
       </c>
       <c r="C20" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G20, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G20)),HYPERLINK(Sheet1!G20, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E21, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E21)),HYPERLINK(Sheet1!E21, "link"),"")</f>
+        <v/>
       </c>
       <c r="B21" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F21, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F21)),HYPERLINK(Sheet1!F21, "link"),"")</f>
+        <v/>
       </c>
       <c r="C21" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G21, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G21)),HYPERLINK(Sheet1!G21, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E22, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E22)),HYPERLINK(Sheet1!E22, "link"),"")</f>
+        <v/>
       </c>
       <c r="B22" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F22, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F22)),HYPERLINK(Sheet1!F22, "link"),"")</f>
+        <v/>
       </c>
       <c r="C22" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G22, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G22)),HYPERLINK(Sheet1!G22, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E23, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E23)),HYPERLINK(Sheet1!E23, "link"),"")</f>
+        <v/>
       </c>
       <c r="B23" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F23, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F23)),HYPERLINK(Sheet1!F23, "link"),"")</f>
+        <v/>
       </c>
       <c r="C23" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G23, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G23)),HYPERLINK(Sheet1!G23, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E24, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E24)),HYPERLINK(Sheet1!E24, "link"),"")</f>
+        <v/>
       </c>
       <c r="B24" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F24, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F24)),HYPERLINK(Sheet1!F24, "link"),"")</f>
+        <v/>
       </c>
       <c r="C24" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G24, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G24)),HYPERLINK(Sheet1!G24, "link"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="str">
-        <f>HYPERLINK(Sheet1!E25, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!E25)),HYPERLINK(Sheet1!E25, "link"),"")</f>
+        <v/>
       </c>
       <c r="B25" s="1" t="str">
-        <f>HYPERLINK(Sheet1!F25, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!F25)),HYPERLINK(Sheet1!F25, "link"),"")</f>
+        <v/>
       </c>
       <c r="C25" s="1" t="str">
-        <f>HYPERLINK(Sheet1!G25, "link")</f>
-        <v>link</v>
+        <f>IF(NOT(ISBLANK(Sheet1!G25)),HYPERLINK(Sheet1!G25, "link"),"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>